<commit_message>
Made changes to the converter function
</commit_message>
<xml_diff>
--- a/excel2sbol/tests/test_files/pichia_toolkit_KWK_v002 copy_Prubhtej.xlsx
+++ b/excel2sbol/tests/test_files/pichia_toolkit_KWK_v002 copy_Prubhtej.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ps/venv/Excel-to-SBOL/excel2sbol/tests/test_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B33D05F0-7957-5444-AE58-D8DBC420F52E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4780AD1-A85D-3246-9245-0D8FC9C89F66}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15940" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7734" uniqueCount="7584">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7722" uniqueCount="7584">
   <si>
     <t>Collection Name</t>
   </si>
@@ -22827,7 +22827,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
-  <fonts count="25" x14ac:knownFonts="1">
+  <fonts count="24" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -22965,12 +22965,6 @@
     <font>
       <b/>
       <u/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Arial"/>
@@ -23162,7 +23156,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -23202,7 +23196,6 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
@@ -25183,14 +25176,17 @@
   <dimension ref="A1:M2535"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.28515625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="18.7109375" customWidth="1"/>
     <col min="2" max="2" width="16" customWidth="1"/>
-    <col min="3" max="26" width="10.5703125" customWidth="1"/>
+    <col min="3" max="3" width="10.5703125" customWidth="1"/>
+    <col min="4" max="4" width="34.85546875" customWidth="1"/>
+    <col min="5" max="5" width="60" customWidth="1"/>
+    <col min="6" max="26" width="10.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -25219,7 +25215,7 @@
       <c r="B2" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="34" t="s">
         <v>136</v>
       </c>
       <c r="D2" s="3" t="s">
@@ -25340,7 +25336,7 @@
       <c r="A9" s="3">
         <v>1</v>
       </c>
-      <c r="B9" s="38" t="s">
+      <c r="B9" s="37" t="s">
         <v>71</v>
       </c>
       <c r="C9" s="3" t="s">
@@ -67719,6 +67715,7 @@
     <hyperlink ref="C2372" r:id="rId3" xr:uid="{00000000-0004-0000-0100-000002000000}"/>
     <hyperlink ref="C2518" r:id="rId4" xr:uid="{00000000-0004-0000-0100-000003000000}"/>
     <hyperlink ref="C3" r:id="rId5" xr:uid="{944FC238-C057-EF41-A520-CEE805C1185C}"/>
+    <hyperlink ref="C2" r:id="rId6" xr:uid="{903157F5-B70E-A645-8B30-4DA0031E0851}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>
@@ -69317,7 +69314,7 @@
   <dimension ref="A1:AA21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.28515625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -69385,9 +69382,7 @@
       <c r="G2" s="3"/>
       <c r="H2" s="3"/>
       <c r="I2" s="3"/>
-      <c r="J2" s="39" t="s">
-        <v>7569</v>
-      </c>
+      <c r="J2" s="38"/>
     </row>
     <row r="3" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A3" s="29" t="s">
@@ -69396,13 +69391,13 @@
       <c r="B3" s="3" t="s">
         <v>7560</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="34" t="s">
         <v>7559</v>
       </c>
       <c r="D3" s="37" t="s">
         <v>7581</v>
       </c>
-      <c r="E3" s="38" t="s">
+      <c r="E3" s="37" t="s">
         <v>7582</v>
       </c>
       <c r="F3" s="3" t="b">
@@ -69411,7 +69406,7 @@
       <c r="G3" s="3"/>
       <c r="H3" s="3"/>
       <c r="I3" s="3"/>
-      <c r="J3" s="39" t="s">
+      <c r="J3" s="38" t="s">
         <v>7583</v>
       </c>
     </row>
@@ -69437,9 +69432,7 @@
       <c r="G4" s="3"/>
       <c r="H4" s="3"/>
       <c r="I4" s="3"/>
-      <c r="J4" s="39" t="s">
-        <v>7569</v>
-      </c>
+      <c r="J4" s="38"/>
     </row>
     <row r="5" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A5" s="29" t="s">
@@ -69469,9 +69462,7 @@
       <c r="I5" s="3" t="s">
         <v>7561</v>
       </c>
-      <c r="J5" s="39" t="s">
-        <v>7569</v>
-      </c>
+      <c r="J5" s="38"/>
     </row>
     <row r="6" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A6" s="29" t="s">
@@ -69495,9 +69486,7 @@
       <c r="G6" s="3"/>
       <c r="H6" s="3"/>
       <c r="I6" s="3"/>
-      <c r="J6" s="39" t="s">
-        <v>7569</v>
-      </c>
+      <c r="J6" s="38"/>
     </row>
     <row r="7" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A7" s="29" t="s">
@@ -69518,9 +69507,7 @@
       <c r="F7" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="J7" s="39" t="s">
-        <v>7569</v>
-      </c>
+      <c r="J7" s="38"/>
     </row>
     <row r="8" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A8" s="29" t="s">
@@ -69544,9 +69531,7 @@
       <c r="G8" s="3"/>
       <c r="H8" s="3"/>
       <c r="I8" s="3"/>
-      <c r="J8" s="39" t="s">
-        <v>7569</v>
-      </c>
+      <c r="J8" s="38"/>
       <c r="K8" s="3"/>
       <c r="L8" s="3"/>
       <c r="M8" s="3"/>
@@ -69593,9 +69578,7 @@
       <c r="I9" s="3" t="s">
         <v>7561</v>
       </c>
-      <c r="J9" s="39" t="s">
-        <v>7569</v>
-      </c>
+      <c r="J9" s="38"/>
     </row>
     <row r="10" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A10" s="29" t="s">
@@ -69625,9 +69608,7 @@
       <c r="I10" s="3" t="s">
         <v>7561</v>
       </c>
-      <c r="J10" s="39" t="s">
-        <v>7569</v>
-      </c>
+      <c r="J10" s="38"/>
     </row>
     <row r="11" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A11" s="29" t="s">
@@ -69651,9 +69632,7 @@
       <c r="G11" s="3"/>
       <c r="H11" s="3"/>
       <c r="I11" s="3"/>
-      <c r="J11" s="39" t="s">
-        <v>7569</v>
-      </c>
+      <c r="J11" s="38"/>
     </row>
     <row r="12" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A12" s="29" t="s">
@@ -69677,9 +69656,7 @@
       <c r="G12" s="3"/>
       <c r="H12" s="3"/>
       <c r="I12" s="3"/>
-      <c r="J12" s="39" t="s">
-        <v>7569</v>
-      </c>
+      <c r="J12" s="38"/>
     </row>
     <row r="13" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A13" s="29" t="s">
@@ -69703,9 +69680,7 @@
       <c r="G13" s="3"/>
       <c r="H13" s="3"/>
       <c r="I13" s="3"/>
-      <c r="J13" s="39" t="s">
-        <v>7569</v>
-      </c>
+      <c r="J13" s="38"/>
     </row>
     <row r="14" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A14" s="29" t="s">
@@ -69735,9 +69710,7 @@
       <c r="I14" s="3" t="s">
         <v>7578</v>
       </c>
-      <c r="J14" s="39" t="s">
-        <v>7569</v>
-      </c>
+      <c r="J14" s="38"/>
     </row>
     <row r="21" spans="5:16" x14ac:dyDescent="0.2">
       <c r="E21" s="3"/>
@@ -69760,6 +69733,7 @@
     <hyperlink ref="C6" r:id="rId3" xr:uid="{00000000-0004-0000-0500-000002000000}"/>
     <hyperlink ref="C9" r:id="rId4" xr:uid="{00000000-0004-0000-0500-000003000000}"/>
     <hyperlink ref="C10" r:id="rId5" xr:uid="{00000000-0004-0000-0500-000004000000}"/>
+    <hyperlink ref="C3" r:id="rId6" xr:uid="{8B69CBCA-F6B1-B94B-85F9-58E7F3675B67}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>

</xml_diff>

<commit_message>
Added tyto functionality to the converter
</commit_message>
<xml_diff>
--- a/excel2sbol/tests/test_files/pichia_toolkit_KWK_v002 copy_Prubhtej.xlsx
+++ b/excel2sbol/tests/test_files/pichia_toolkit_KWK_v002 copy_Prubhtej.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ps/venv/Excel-to-SBOL/excel2sbol/tests/test_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4780AD1-A85D-3246-9245-0D8FC9C89F66}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2EE9C4B-98A1-D04F-A221-4D8B92CF7AEA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15940" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7722" uniqueCount="7584">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7725" uniqueCount="7586">
   <si>
     <t>Collection Name</t>
   </si>
@@ -22808,12 +22808,6 @@
     <t>F</t>
   </si>
   <si>
-    <t>Ontology Lookup</t>
-  </si>
-  <si>
-    <t>Ontology Name</t>
-  </si>
-  <si>
     <t xml:space="preserve">                     TRUE</t>
   </si>
   <si>
@@ -22821,6 +22815,18 @@
   </si>
   <si>
     <t>SO</t>
+  </si>
+  <si>
+    <t>NCBITaxon</t>
+  </si>
+  <si>
+    <t>Ontology_Name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                      TRUE</t>
+  </si>
+  <si>
+    <t>Ontology_Lookup</t>
   </si>
 </sst>
 </file>
@@ -23188,16 +23194,16 @@
     <xf numFmtId="0" fontId="18" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="19" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -23600,12 +23606,12 @@
       <c r="J10" s="3"/>
     </row>
     <row r="11" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A11" s="31"/>
-      <c r="B11" s="32"/>
-      <c r="C11" s="32"/>
-      <c r="D11" s="32"/>
-      <c r="E11" s="32"/>
-      <c r="F11" s="33"/>
+      <c r="A11" s="36"/>
+      <c r="B11" s="37"/>
+      <c r="C11" s="37"/>
+      <c r="D11" s="37"/>
+      <c r="E11" s="37"/>
+      <c r="F11" s="38"/>
       <c r="G11" s="3"/>
       <c r="H11" s="3"/>
       <c r="I11" s="3"/>
@@ -25215,7 +25221,7 @@
       <c r="B2" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="C2" s="34" t="s">
+      <c r="C2" s="31" t="s">
         <v>136</v>
       </c>
       <c r="D2" s="3" t="s">
@@ -25234,7 +25240,7 @@
       <c r="B3" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="C3" s="34" t="s">
+      <c r="C3" s="31" t="s">
         <v>138</v>
       </c>
       <c r="D3" s="3" t="s">
@@ -25336,7 +25342,7 @@
       <c r="A9" s="3">
         <v>1</v>
       </c>
-      <c r="B9" s="37" t="s">
+      <c r="B9" s="34" t="s">
         <v>71</v>
       </c>
       <c r="C9" s="3" t="s">
@@ -69079,7 +69085,7 @@
   <dimension ref="A1:F14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="O31" sqref="O31"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.28515625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -69314,7 +69320,7 @@
   <dimension ref="A1:AA21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J3" sqref="J3"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.28515625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -69338,8 +69344,8 @@
       <c r="C1" s="21" t="s">
         <v>7552</v>
       </c>
-      <c r="D1" s="35" t="s">
-        <v>7579</v>
+      <c r="D1" s="32" t="s">
+        <v>7585</v>
       </c>
       <c r="E1" s="21" t="s">
         <v>7553</v>
@@ -69356,8 +69362,8 @@
       <c r="I1" s="21" t="s">
         <v>7557</v>
       </c>
-      <c r="J1" s="36" t="s">
-        <v>7580</v>
+      <c r="J1" s="33" t="s">
+        <v>7583</v>
       </c>
     </row>
     <row r="2" spans="1:27" x14ac:dyDescent="0.2">
@@ -69370,7 +69376,7 @@
       <c r="C2" s="3" t="s">
         <v>7559</v>
       </c>
-      <c r="D2" s="37" t="b">
+      <c r="D2" s="34" t="b">
         <v>0</v>
       </c>
       <c r="E2" s="3" t="b">
@@ -69382,7 +69388,7 @@
       <c r="G2" s="3"/>
       <c r="H2" s="3"/>
       <c r="I2" s="3"/>
-      <c r="J2" s="38"/>
+      <c r="J2" s="35"/>
     </row>
     <row r="3" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A3" s="29" t="s">
@@ -69391,14 +69397,14 @@
       <c r="B3" s="3" t="s">
         <v>7560</v>
       </c>
-      <c r="C3" s="34" t="s">
+      <c r="C3" s="31" t="s">
         <v>7559</v>
       </c>
-      <c r="D3" s="37" t="s">
-        <v>7581</v>
-      </c>
-      <c r="E3" s="37" t="s">
-        <v>7582</v>
+      <c r="D3" s="34" t="s">
+        <v>7579</v>
+      </c>
+      <c r="E3" s="34" t="s">
+        <v>7580</v>
       </c>
       <c r="F3" s="3" t="b">
         <v>0</v>
@@ -69406,8 +69412,8 @@
       <c r="G3" s="3"/>
       <c r="H3" s="3"/>
       <c r="I3" s="3"/>
-      <c r="J3" s="38" t="s">
-        <v>7583</v>
+      <c r="J3" s="35" t="s">
+        <v>7581</v>
       </c>
     </row>
     <row r="4" spans="1:27" x14ac:dyDescent="0.2">
@@ -69420,7 +69426,7 @@
       <c r="C4" s="22" t="s">
         <v>7563</v>
       </c>
-      <c r="D4" s="37" t="b">
+      <c r="D4" s="34" t="b">
         <v>0</v>
       </c>
       <c r="E4" s="3" t="b">
@@ -69432,7 +69438,7 @@
       <c r="G4" s="3"/>
       <c r="H4" s="3"/>
       <c r="I4" s="3"/>
-      <c r="J4" s="38"/>
+      <c r="J4" s="35"/>
     </row>
     <row r="5" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A5" s="29" t="s">
@@ -69444,7 +69450,7 @@
       <c r="C5" s="25" t="s">
         <v>7563</v>
       </c>
-      <c r="D5" s="37" t="b">
+      <c r="D5" s="34" t="b">
         <v>0</v>
       </c>
       <c r="E5" s="3" t="b">
@@ -69462,7 +69468,7 @@
       <c r="I5" s="3" t="s">
         <v>7561</v>
       </c>
-      <c r="J5" s="38"/>
+      <c r="J5" s="35"/>
     </row>
     <row r="6" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A6" s="29" t="s">
@@ -69474,7 +69480,7 @@
       <c r="C6" s="25" t="s">
         <v>7568</v>
       </c>
-      <c r="D6" s="37" t="b">
+      <c r="D6" s="34" t="b">
         <v>0</v>
       </c>
       <c r="E6" s="3" t="b">
@@ -69486,7 +69492,7 @@
       <c r="G6" s="3"/>
       <c r="H6" s="3"/>
       <c r="I6" s="3"/>
-      <c r="J6" s="38"/>
+      <c r="J6" s="35"/>
     </row>
     <row r="7" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A7" s="29" t="s">
@@ -69498,7 +69504,7 @@
       <c r="C7" s="3" t="s">
         <v>7569</v>
       </c>
-      <c r="D7" s="37" t="b">
+      <c r="D7" s="34" t="b">
         <v>0</v>
       </c>
       <c r="E7" s="3" t="b">
@@ -69507,7 +69513,7 @@
       <c r="F7" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="J7" s="38"/>
+      <c r="J7" s="35"/>
     </row>
     <row r="8" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A8" s="29" t="s">
@@ -69519,7 +69525,7 @@
       <c r="C8" s="3" t="s">
         <v>7569</v>
       </c>
-      <c r="D8" s="37" t="b">
+      <c r="D8" s="34" t="b">
         <v>0</v>
       </c>
       <c r="E8" s="3" t="b">
@@ -69531,7 +69537,7 @@
       <c r="G8" s="3"/>
       <c r="H8" s="3"/>
       <c r="I8" s="3"/>
-      <c r="J8" s="38"/>
+      <c r="J8" s="35"/>
       <c r="K8" s="3"/>
       <c r="L8" s="3"/>
       <c r="M8" s="3"/>
@@ -69560,8 +69566,8 @@
       <c r="C9" s="25" t="s">
         <v>7563</v>
       </c>
-      <c r="D9" s="37" t="b">
-        <v>0</v>
+      <c r="D9" s="34" t="b">
+        <v>1</v>
       </c>
       <c r="E9" s="3" t="b">
         <v>1</v>
@@ -69578,7 +69584,9 @@
       <c r="I9" s="3" t="s">
         <v>7561</v>
       </c>
-      <c r="J9" s="38"/>
+      <c r="J9" t="s">
+        <v>7582</v>
+      </c>
     </row>
     <row r="10" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A10" s="29" t="s">
@@ -69587,11 +69595,11 @@
       <c r="B10" s="3" t="s">
         <v>7572</v>
       </c>
-      <c r="C10" s="25" t="s">
+      <c r="C10" s="31" t="s">
         <v>7563</v>
       </c>
-      <c r="D10" s="37" t="b">
-        <v>0</v>
+      <c r="D10" s="34" t="s">
+        <v>7584</v>
       </c>
       <c r="E10" s="3" t="b">
         <v>1</v>
@@ -69608,7 +69616,9 @@
       <c r="I10" s="3" t="s">
         <v>7561</v>
       </c>
-      <c r="J10" s="38"/>
+      <c r="J10" t="s">
+        <v>7582</v>
+      </c>
     </row>
     <row r="11" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A11" s="29" t="s">
@@ -69620,7 +69630,7 @@
       <c r="C11" s="3" t="s">
         <v>7559</v>
       </c>
-      <c r="D11" s="37" t="b">
+      <c r="D11" s="34" t="b">
         <v>0</v>
       </c>
       <c r="E11" s="3" t="b">
@@ -69632,7 +69642,7 @@
       <c r="G11" s="3"/>
       <c r="H11" s="3"/>
       <c r="I11" s="3"/>
-      <c r="J11" s="38"/>
+      <c r="J11" s="35"/>
     </row>
     <row r="12" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A12" s="29" t="s">
@@ -69644,7 +69654,7 @@
       <c r="C12" s="3" t="s">
         <v>7569</v>
       </c>
-      <c r="D12" s="37" t="b">
+      <c r="D12" s="34" t="b">
         <v>0</v>
       </c>
       <c r="E12" s="3" t="b">
@@ -69656,7 +69666,7 @@
       <c r="G12" s="3"/>
       <c r="H12" s="3"/>
       <c r="I12" s="3"/>
-      <c r="J12" s="38"/>
+      <c r="J12" s="35"/>
     </row>
     <row r="13" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A13" s="29" t="s">
@@ -69668,7 +69678,7 @@
       <c r="C13" s="3" t="s">
         <v>7559</v>
       </c>
-      <c r="D13" s="37" t="b">
+      <c r="D13" s="34" t="b">
         <v>0</v>
       </c>
       <c r="E13" s="3" t="b">
@@ -69680,7 +69690,7 @@
       <c r="G13" s="3"/>
       <c r="H13" s="3"/>
       <c r="I13" s="3"/>
-      <c r="J13" s="38"/>
+      <c r="J13" s="35"/>
     </row>
     <row r="14" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A14" s="29" t="s">
@@ -69692,7 +69702,7 @@
       <c r="C14" s="24" t="s">
         <v>7576</v>
       </c>
-      <c r="D14" s="37" t="b">
+      <c r="D14" s="34" t="b">
         <v>0</v>
       </c>
       <c r="E14" s="3" t="b">
@@ -69710,7 +69720,7 @@
       <c r="I14" s="3" t="s">
         <v>7578</v>
       </c>
-      <c r="J14" s="38"/>
+      <c r="J14" s="35"/>
     </row>
     <row r="21" spans="5:16" x14ac:dyDescent="0.2">
       <c r="E21" s="3"/>

</xml_diff>